<commit_message>
shapiro and chi tests explained
</commit_message>
<xml_diff>
--- a/testing/chi_test.xlsx
+++ b/testing/chi_test.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40011956\Desktop\Deep_Learning_Liver_Prediction\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\Desktop\Deep_Learning_Liver_Prediction\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DA8562-6BD9-43DB-8ED2-6524D866A0F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>gender</t>
   </si>
@@ -89,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,7 +207,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -820,7 +828,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -927,7 +934,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1505,7 +1511,552 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>p values</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SPANISH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$23:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>gender</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>diabetes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dyalisis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>etiology</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>portal thrombosis</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tips</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>hepatorhenal syndrome</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>donor gender</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>arterial hypertension</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>casue of death</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>hypotension</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>inotropes</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>multi organic tx</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>combined tx</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>partial/incomplete graft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$23:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.88770000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79910000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8738999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1658</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.51439999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97950000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98819999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.55759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.64359999999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-76C2-41AE-87B1-5FD6C57208A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BRITISH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$23:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>gender</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>diabetes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dyalisis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>etiology</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>portal thrombosis</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tips</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>hepatorhenal syndrome</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>donor gender</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>arterial hypertension</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>casue of death</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>hypotension</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>inotropes</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>multi organic tx</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>combined tx</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>partial/incomplete graft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$23:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.9859</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76349999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51439999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27460000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.51439999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99929999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.60089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.47160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.91069999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.47160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.60089999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-76C2-41AE-87B1-5FD6C57208A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="404921896"/>
+        <c:axId val="404916976"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="404921896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404916976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="404916976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404921896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1649,6 +2200,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2655,24 +3246,533 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>36195</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>97155</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2689,20 +3789,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>95983</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>339090</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>73123</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>512885</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>172183</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>32825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>149323</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2712,6 +3818,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA2406AE-44ED-4471-86B9-E1B73DAE654F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2982,19 +4124,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3004,7 +4146,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3018,7 +4160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -3044,7 +4186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3063,7 +4205,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -3093,7 +4235,7 @@
         <v>7.0000999999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -3123,7 +4265,7 @@
         <v>0.99989999999999668</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -3153,7 +4295,7 @@
         <v>42.999899999999997</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -3183,7 +4325,7 @@
         <v>33.16340000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -3213,7 +4355,7 @@
         <v>3.8570999999999955</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -3243,7 +4385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -3273,7 +4415,7 @@
         <v>1.0000000000331966E-4</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -3303,7 +4445,7 @@
         <v>6.9999000000000002</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -3333,7 +4475,7 @@
         <v>17.999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -3363,7 +4505,7 @@
         <v>9.0546000000000006</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -3393,7 +4535,7 @@
         <v>1.9998000000000005</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -3423,7 +4565,7 @@
         <v>5.0000999999999998</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -3453,7 +4595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="I19" t="s">
         <v>17</v>
       </c>
@@ -3468,7 +4610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="I20" t="s">
         <v>18</v>
       </c>
@@ -3481,6 +4623,179 @@
       <c r="L20">
         <f t="shared" si="0"/>
         <v>40.999899999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.88770000000000004</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.9859</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.79910000000000003</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.76349999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.51439999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.8738999999999999</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.1658</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.27460000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.51439999999999997</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.51439999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.83179999999999998</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.83179999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.97950000000000004</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.99929999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.99619999999999997</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.60089999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.98819999999999997</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.55759999999999998</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.47160000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.99990000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.91069999999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.64359999999999995</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.47160000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.60089999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>